<commit_message>
Update ATD05 Beregn markedsføringsbidrag.xlsx
</commit_message>
<xml_diff>
--- a/05 Test/ATD05 Beregn markedsføringsbidrag.xlsx
+++ b/05 Test/ATD05 Beregn markedsføringsbidrag.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelvi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benky\OneDrive\IdeaProjects\HoeKulator\05 Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D6C8E08-C955-4DCA-960E-FFC80598D55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="13_ncr:1_{6D6C8E08-C955-4DCA-960E-FFC80598D55E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6FCB507A-43BD-4A7F-A887-BC11F488CD18}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{85BF57BC-2068-44D8-8316-5DD049F8480B}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="51">
   <si>
     <t>Test Data</t>
   </si>
@@ -177,15 +177,21 @@
   </si>
   <si>
     <t>BF = 500,493</t>
+  </si>
+  <si>
+    <t>Main succes scenario</t>
+  </si>
+  <si>
+    <t>BF = 14640</t>
+  </si>
+  <si>
+    <t>SFO = 1880</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -241,7 +247,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -386,6 +392,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -394,7 +420,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="3" applyBorder="1"/>
@@ -432,16 +458,16 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="5" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -762,10 +788,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15EF9607-4FB9-4C4D-ACC9-E0278E529E2D}">
-  <dimension ref="A2:G25"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -813,14 +839,14 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>30</v>
+      <c r="D4" s="17" t="s">
+        <v>48</v>
       </c>
       <c r="F4" s="27" t="s">
         <v>22</v>
@@ -830,14 +856,14 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="30">
-        <v>4750000</v>
-      </c>
-      <c r="D5" s="14"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="36">
+        <v>12760</v>
+      </c>
+      <c r="D5" s="19"/>
       <c r="F5" s="27" t="s">
         <v>39</v>
       </c>
@@ -846,17 +872,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="15" t="s">
-        <v>21</v>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>30</v>
       </c>
       <c r="F6" s="27" t="s">
         <v>40</v>
@@ -866,11 +890,13 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="B7" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="14"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="30">
+        <v>4750000</v>
+      </c>
       <c r="D7" s="14"/>
       <c r="F7" s="27" t="s">
         <v>41</v>
@@ -880,150 +906,147 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="22" t="s">
-        <v>20</v>
+      <c r="A8" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="D8" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="20" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="16" t="s">
+      <c r="C11" s="21"/>
+      <c r="D11" s="14"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B12" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="C12" s="17" t="s">
         <v>26</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="18"/>
-      <c r="B11" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="19"/>
-      <c r="D11" s="14"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>27</v>
       </c>
       <c r="D12" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="23" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="19"/>
+      <c r="D13" s="14"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="14"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="16"/>
-      <c r="B14" s="15" t="s">
+      <c r="C15" s="4"/>
+      <c r="D15" s="14"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="16"/>
+      <c r="B16" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="C16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D16" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="18"/>
-      <c r="B15" s="14" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18"/>
+      <c r="B17" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="25">
+      <c r="C17" s="25">
         <f>1000 - 500.49</f>
         <v>499.51</v>
       </c>
-      <c r="D15" s="14"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="D17" s="14"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9" t="s">
+      <c r="B18" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C18" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="3"/>
-      <c r="B17" s="23" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C19" s="26">
         <f>500.49 - 1000</f>
         <v>-499.51</v>
       </c>
-      <c r="D17" s="14"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="16"/>
-      <c r="B18" s="15" t="s">
+      <c r="D19" s="14"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="16"/>
+      <c r="B20" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="18"/>
-      <c r="B19" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="31">
-        <f>1000-500.499</f>
-        <v>499.50099999999998</v>
-      </c>
-      <c r="D19" s="14"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="17" t="s">
         <v>40</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -1031,21 +1054,23 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="34">
-        <f>SUM(500.499-1000)</f>
-        <v>-499.50099999999998</v>
+      <c r="A21" s="18"/>
+      <c r="B21" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="31">
+        <v>499.5</v>
       </c>
       <c r="D21" s="14"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="24" t="s">
         <v>40</v>
       </c>
       <c r="D22" s="15" t="s">
@@ -1053,35 +1078,56 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="32">
+        <v>-499.5</v>
+      </c>
+      <c r="D23" s="14"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B24" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C25" s="31">
         <f>1000-500.493</f>
         <v>499.50700000000001</v>
       </c>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B24" s="9" t="s">
+      <c r="D25" s="14"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C26" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D26" s="15" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B25" s="23" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="33">
+      <c r="C27" s="32">
         <f>SUM(500.493-1000)</f>
         <v>-499.50700000000001</v>
       </c>
-      <c r="D25" s="14"/>
+      <c r="D27" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>